<commit_message>
Fix bags in delivery price
</commit_message>
<xml_diff>
--- a/vectortool_customers/customers.xlsx
+++ b/vectortool_customers/customers.xlsx
@@ -398,7 +398,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
       <selection activeCell="A58" sqref="A58"/>
@@ -998,6 +998,18 @@
         </is>
       </c>
     </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>ХЕЧ ТЕК</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>ХЕЧ ТЕК Україна</t>
+        </is>
+      </c>
+    </row>
     <row r="52" ht="15" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>